<commit_message>
operacion and y bin dec hex
</commit_message>
<xml_diff>
--- a/docs/layer-3.xlsx
+++ b/docs/layer-3.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-m17\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A711345C-E9A7-4C4F-8190-7A53DFD9D183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4280556-EF71-4F3C-A317-478C206B0E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" xr2:uid="{D58E1B7F-9D53-4143-8877-B1E8AC398FDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{D58E1B7F-9D53-4143-8877-B1E8AC398FDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
+    <sheet name="AND" sheetId="2" r:id="rId2"/>
+    <sheet name="BINARIO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="136">
   <si>
     <t>10.54.11.25</t>
   </si>
@@ -169,13 +172,442 @@
   </si>
   <si>
     <t>10.224.0.48</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>ip</t>
+  </si>
+  <si>
+    <t>mask</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>Byte 1</t>
+  </si>
+  <si>
+    <t>Byte 2</t>
+  </si>
+  <si>
+    <t>Byte 3</t>
+  </si>
+  <si>
+    <t>Byte 4</t>
+  </si>
+  <si>
+    <t>192.168.0.10</t>
+  </si>
+  <si>
+    <t>11000000</t>
+  </si>
+  <si>
+    <t>10101000</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>00001010</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>11111111</t>
+  </si>
+  <si>
+    <t>BINARIO</t>
+  </si>
+  <si>
+    <t>DEC</t>
+  </si>
+  <si>
+    <t>2^0</t>
+  </si>
+  <si>
+    <t>2^1</t>
+  </si>
+  <si>
+    <t>2^6</t>
+  </si>
+  <si>
+    <t>2^5</t>
+  </si>
+  <si>
+    <t>2^4</t>
+  </si>
+  <si>
+    <t>2^3</t>
+  </si>
+  <si>
+    <t>2^2</t>
+  </si>
+  <si>
+    <t>2^7</t>
+  </si>
+  <si>
+    <t>192.168.0.0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>111111</t>
+    </r>
+  </si>
+  <si>
+    <t>Solo se mantienen encendidos los bits que se encuentran en 1 tanto en la direccion ip como en la mascara de subred, caso contrario quedara en 0. Se utiliza para determinar la direccion de red y por consecuente la direccion de broadcast.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>111</t>
+    </r>
+  </si>
+  <si>
+    <t>192.168.0.255</t>
+  </si>
+  <si>
+    <t>BIN</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>VAL</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>HEX</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>00000010</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>00000011</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>00000100</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>00000101</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>00000110</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>00000111</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>00001000</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>00001001</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>00001011</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>00001100</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>00001101</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>00001110</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>00001111</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>00010000</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>00011001</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>01100011</t>
+  </si>
+  <si>
+    <t>0x63</t>
+  </si>
+  <si>
+    <t>01100100</t>
+  </si>
+  <si>
+    <t>0x64</t>
+  </si>
+  <si>
+    <t>0xFF</t>
+  </si>
+  <si>
+    <t>0x256</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0x7B6</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>10^2</t>
+  </si>
+  <si>
+    <t>10^1</t>
+  </si>
+  <si>
+    <t>10^0</t>
+  </si>
+  <si>
+    <t>16^3</t>
+  </si>
+  <si>
+    <t>16^2</t>
+  </si>
+  <si>
+    <t>16^1</t>
+  </si>
+  <si>
+    <t>16^0</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,13 +621,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -210,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -218,104 +697,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="21">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -425,6 +890,100 @@
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -439,17 +998,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7CE3BD4E-2E43-4A46-8837-F60AF8B83C77}" name="Tabla8" displayName="Tabla8" ref="A1:F15" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7CE3BD4E-2E43-4A46-8837-F60AF8B83C77}" name="Tabla8" displayName="Tabla8" ref="A1:F15" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:F15" xr:uid="{7CE3BD4E-2E43-4A46-8837-F60AF8B83C77}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0417635E-5AAA-4124-BF24-E685028B28E9}" name="Packet" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{EDF60D3F-1116-4F5F-9918-E6A264736379}" name="10.54.11.25" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{8BB3DE53-8464-4FC4-8ED3-1BBD215DC785}" name="10.32.45.11" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{005EF067-1823-48DB-B2F2-5667F5E88485}" name="10.8.25.5" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{6AF70F22-B26D-4526-A388-B2BBF852BE08}" name="10.57.10.90" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{BD81082D-82F6-428E-B38C-44BBC664C33B}" name="10.224.0.56" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{0417635E-5AAA-4124-BF24-E685028B28E9}" name="Packet" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{EDF60D3F-1116-4F5F-9918-E6A264736379}" name="10.54.11.25" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{8BB3DE53-8464-4FC4-8ED3-1BBD215DC785}" name="10.32.45.11" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{005EF067-1823-48DB-B2F2-5667F5E88485}" name="10.8.25.5" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{6AF70F22-B26D-4526-A388-B2BBF852BE08}" name="10.57.10.90" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{BD81082D-82F6-428E-B38C-44BBC664C33B}" name="10.224.0.56" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4354FB12-22FC-4071-ACE3-8C4D19BD5E2E}" name="Tabla1" displayName="Tabla1" ref="H1:I10" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="H1:I10" xr:uid="{4354FB12-22FC-4071-ACE3-8C4D19BD5E2E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{1271DDA5-9E86-48E8-A07E-AEBCABE3991F}" name="BINARIO" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{AECF3B72-B0B0-4A35-9286-6BC6AC8AFDB0}" name="DEC" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CF580A89-3C58-47FF-B9C1-271230B2676F}" name="Tabla2" displayName="Tabla2" ref="A1:F5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+  <autoFilter ref="A1:F5" xr:uid="{CF580A89-3C58-47FF-B9C1-271230B2676F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{774A2505-7684-4EF6-9C99-FC97C5A754B9}" name="AND" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{47531761-5CE6-4050-B64F-CD949926EA0B}" name="DEC" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{841295DD-8505-44A3-8375-C709086C057D}" name="Byte 1" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{2B56BD6B-F0A4-442E-A555-2940984138FE}" name="Byte 2" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{B3D3BD95-92B6-4B5D-8866-87091C3AF73C}" name="Byte 3" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{129EF05C-798B-4504-BA3B-736F82355F6B}" name="Byte 4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FB202A22-8BB6-41B0-BCE6-20435DC7D2FB}" name="Tabla3" displayName="Tabla3" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22" xr:uid="{FB202A22-8BB6-41B0-BCE6-20435DC7D2FB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C3E71064-D1A7-4436-8D3B-24547A016B88}" name="DEC" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{605ED81F-7F71-4091-B439-2A9B0AC9E520}" name="BIN" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{A3B3E7A6-1EB2-4115-B1A5-309E782D032D}" name="HEX" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -752,7 +1349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18B0A77-27C2-4351-B317-1425992024F1}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1076,4 +1673,919 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73B2EDE-56B1-4A37-8CE7-15B1C789EE22}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="3">
+        <v>11000000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="3">
+        <v>11100000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="3">
+        <v>11110000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="H7" s="3">
+        <v>11111000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="H8" s="3">
+        <v>11111100</v>
+      </c>
+      <c r="I8" s="1">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="H9" s="3">
+        <v>11111110</v>
+      </c>
+      <c r="I9" s="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="3">
+        <v>11111111</v>
+      </c>
+      <c r="I10" s="1">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:F10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DD203D-5998-4C26-AE4D-341BF5E6AC73}">
+  <dimension ref="A1:AE22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="3" customWidth="1"/>
+    <col min="5" max="31" width="5" customWidth="1"/>
+    <col min="32" max="36" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="8">
+        <f>10^3</f>
+        <v>1000</v>
+      </c>
+      <c r="G2" s="9">
+        <f>10^2</f>
+        <v>100</v>
+      </c>
+      <c r="H2" s="8">
+        <f>10^1</f>
+        <v>10</v>
+      </c>
+      <c r="I2" s="9">
+        <f>10^0</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="11">
+        <f>2^7</f>
+        <v>128</v>
+      </c>
+      <c r="M2" s="7">
+        <f>2^6</f>
+        <v>64</v>
+      </c>
+      <c r="N2" s="11">
+        <f>2^5</f>
+        <v>32</v>
+      </c>
+      <c r="O2" s="7">
+        <f>2^4</f>
+        <v>16</v>
+      </c>
+      <c r="P2" s="11">
+        <f>2^3</f>
+        <v>8</v>
+      </c>
+      <c r="Q2" s="7">
+        <f>2^2</f>
+        <v>4</v>
+      </c>
+      <c r="R2" s="11">
+        <f>2^1</f>
+        <v>2</v>
+      </c>
+      <c r="S2" s="7">
+        <f>2^0</f>
+        <v>1</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="V2" s="8">
+        <f>16^3</f>
+        <v>4096</v>
+      </c>
+      <c r="W2" s="9">
+        <f>16^2</f>
+        <v>256</v>
+      </c>
+      <c r="X2" s="8">
+        <f>16^1</f>
+        <v>16</v>
+      </c>
+      <c r="Y2" s="9">
+        <f>16^0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="9">
+        <v>1</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0</v>
+      </c>
+      <c r="O3" s="9">
+        <v>1</v>
+      </c>
+      <c r="P3" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>1</v>
+      </c>
+      <c r="R3" s="8">
+        <v>1</v>
+      </c>
+      <c r="S3" s="9">
+        <v>0</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="S5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" s="14">
+        <f>SUM(T7:AE7)</f>
+        <v>1974</v>
+      </c>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="T6" s="8">
+        <v>0</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="V6" s="8">
+        <v>1</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD6" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="11">
+        <v>512</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="7">
+        <v>64</v>
+      </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="7">
+        <v>16</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7" s="7">
+        <v>4</v>
+      </c>
+      <c r="P7" s="11">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="S7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="T7" s="11"/>
+      <c r="U7" s="15">
+        <v>1024</v>
+      </c>
+      <c r="V7" s="11">
+        <v>512</v>
+      </c>
+      <c r="W7" s="7">
+        <v>256</v>
+      </c>
+      <c r="X7" s="11">
+        <v>128</v>
+      </c>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="11">
+        <v>32</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>16</v>
+      </c>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="7">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="11">
+        <v>2</v>
+      </c>
+      <c r="AE7" s="7"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="14">
+        <f>SUM(F7:Q7)</f>
+        <v>598</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="S8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>25</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>99</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>100</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>255</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="T5:AE5"/>
+    <mergeCell ref="T8:AE8"/>
+    <mergeCell ref="F5:Q5"/>
+    <mergeCell ref="F8:Q8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>